<commit_message>
-Updated the UML diagram for AddMovies and Movies[]
</commit_message>
<xml_diff>
--- a/Exam1 UML Diagrams.xlsx
+++ b/Exam1 UML Diagrams.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bmorledge-hampton19\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\General\Repos\Exam 1 Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -86,10 +86,10 @@
     <t xml:space="preserve"> -PopcornPrice: int</t>
   </si>
   <si>
-    <t xml:space="preserve"> +AddMovie(Movie: newMovie&amp;): void</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -Movie: Movies[100]</t>
+    <t xml:space="preserve"> +AddMovie(Movie: newMovie&amp;): bool </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -Movie: Movies[24]</t>
   </si>
 </sst>
 </file>
@@ -585,7 +585,7 @@
   <dimension ref="B1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>